<commit_message>
fix id filter and prompt func
</commit_message>
<xml_diff>
--- a/assets/translate_prompt.xlsx
+++ b/assets/translate_prompt.xlsx
@@ -45,218 +45,158 @@
     <t>acc</t>
   </si>
   <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
+    <t>loose</t>
+  </si>
+  <si>
+    <t>acc_original</t>
+  </si>
+  <si>
+    <t>loose_original</t>
+  </si>
+  <si>
+    <t>KR_loose</t>
+  </si>
+  <si>
+    <t>KR_acc</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
 Hãy chuyển ngữ văn bản sau đây từ tiếng Trung sang tiếng Việt với độ chính xác cao, giữ gần nhất có thể với văn phong và cấu trúc nguyên gốc. 
-{count_info} 
 Dịch sát nghĩa từng câu, truyền tải đầy đủ thông tin từ bản gốc. Giữ nguyên các tham chiếu văn hóa và thuật ngữ đặc thù mà không cần địa phương hóa quá mức. 
 Đối với tên nhân vật, hãy chuyển sang phát âm tiếng Nhật, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
 Phải dịch TOÀN BỘ văn bản sang tiếng Việt, không được để sót bất kỳ từ/câu tiếng Trung nào chưa dịch.
-Không thêm bớt, không làm thay đổi ý nghĩa của văn bản gốc, tránh diễn giải theo ý riêng. 
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...). 
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và dịch thuật các light novel Nhật Bản sang tiếng Việt. 
-Hãy chuyển ngữ văn bản sau đây từ tiếng Nhật sang tiếng Việt với độ chính xác cao, giữ gần nhất có thể với văn phong và cấu trúc nguyên gốc. 
-{count_info} 
-Ưu tiên tính chính xác và trung thành với nội dung gốc. Cố gắng giữ nguyên cách diễn đạt, nhịp điệu và phong cách của tác giả. 
-Giữ nguyên các tham chiếu văn hóa và thuật ngữ đặc thù mà không cần địa phương hóa quá mức. 
-Giữ nguyên các hậu tố xưng hô như -san, -kun, -chan, -sama, -sensei, v.v. nếu có trong bản gốc
-Không thêm bớt, không làm thay đổi ý nghĩa của văn bản gốc, tránh diễn giải theo ý riêng. 
-Phải dịch TOÀN BỘ văn bản sang tiếng Việt, không được để sót bất kỳ từ/câu tiếng Nhật nào chưa dịch.
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...)
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và dịch thuật các tác phẩm văn học tiếng Anh sang tiếng Việt. 
-Hãy chuyển ngữ văn bản sau đây từ tiếng Anh sang tiếng Việt với độ chính xác cao, giữ gần nhất có thể với văn phong và cấu trúc nguyên gốc. 
-{count_info} 
-Dịch sát nghĩa từng câu, truyền tải đầy đủ thông tin từ bản gốc. 
-Giữ nguyên tên nhân vật, địa danh và các thuật ngữ đặc thù như trong bản gốc tiếng Anh.
-Các thành ngữ, tục ngữ tiếng Anh cần được dịch sang những biểu đạt tương đương trong tiếng Việt nếu có.
-Không thêm bớt, không làm thay đổi ý nghĩa của văn bản gốc, tránh diễn giải theo ý riêng. 
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...)
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và dịch thuật các tác phẩm văn học Hàn Quốc sang tiếng Việt. 
-Hãy chuyển ngữ văn bản sau đây từ tiếng Hàn sang tiếng Việt với độ chính xác cao, giữ gần nhất có thể với văn phong và cấu trúc nguyên gốc. 
-{count_info} 
-Dịch sát nghĩa từng câu, truyền tải đầy đủ thông tin từ bản gốc. 
-Đối với tên nhân vật, hãy chuyển sang phiên âm tiếng Việt theo cách đọc tiếng Hàn.
-Các thuật ngữ đặc trưng văn hóa Hàn Quốc hãy giữ nguyên và thêm giải thích ngắn nếu cần thiết.
-Các mức độ kính ngữ trong tiếng Hàn cần được chuyển thành biểu đạt tương ứng với ngôn ngữ tiếng Việt.
-Không thêm bớt, không làm thay đổi ý nghĩa của văn bản gốc, tránh diễn giải theo ý riêng. 
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...)
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>You are an experienced literary editor specializing in processing and translating Vietnamese literary works into English.
-Please translate the following text from Vietnamese to English with high accuracy, maintaining as closely as possible the original style and structure.
-{count_info}
-Translate each sentence faithfully, conveying complete information from the original text.
-Preserve character names, place names, and specific terminology as they appear in the original Vietnamese.
-Vietnamese idioms and proverbs should be translated into equivalent English expressions where available.
-Do not add or omit content, do not alter the meaning of the original text, and avoid personal interpretation.
-Maintain the original numbering format (1., 2., ...)
-Here is the text to be translated:
-{text}</t>
-  </si>
-  <si>
-    <t>loose</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
-Hãy chuyển ngữ văn bản sau đây từ tiếng Trung sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
-{count_info} 
-Ưu tiên sự tự nhiên và vẻ đẹp của ngôn ngữ tiếng Việt hơn là dịch sát nghĩa từng câu. 
-Đối với tên nhân vật, hãy chuyển sang phát âm tiếng Nhật, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
-Bạn có thể điều chỉnh cấu trúc câu để tạo nhịp điệu đọc tốt hơn, miễn là không làm mất ý nghĩa gốc. 
-Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản. 
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...). 
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
-Hãy chuyển ngữ văn bản sau đây từ tiếng Nhật sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
-{count_info} 
-Ưu tiên sự tự nhiên và vẻ đẹp của ngôn ngữ tiếng Việt hơn là dịch sát nghĩa từng câu. 
-Đối với tên nhân vật, hãy chuyển sang phát âm tiếng Nhật, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
-Bạn có thể điều chỉnh cấu trúc câu để tạo nhịp điệu đọc tốt hơn, miễn là không làm mất ý nghĩa gốc.
-Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản. 
-Phải dịch TOÀN BỘ văn bản sang tiếng Việt, không được để sót bất kỳ từ/câu tiếng Nhật nào chưa dịch.
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...)
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
-Hãy chuyển ngữ văn bản sau đây từ tiếng Anh sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
-{count_info} 
-Ưu tiên sự tự nhiên và vẻ đẹp của ngôn ngữ tiếng Việt hơn là dịch sát nghĩa từng câu. 
-Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản. 
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...)
-Đây là văn bản cần chuyển ngữ:
-{text}
-)</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các tác phẩm văn học Hàn Quốc sang tiếng Việt. 
-Hãy chuyển ngữ văn bản sau đây từ tiếng Hàn sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
-{count_info} 
-Ưu tiên sự tự nhiên và vẻ đẹp của ngôn ngữ tiếng Việt hơn là dịch sát nghĩa từng câu. 
-Đối với tên nhân vật, hãy chuyển sang phiên âm tiếng Việt theo cách đọc tiếng Hàn, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
-Bạn có thể điều chỉnh cấu trúc câu để tạo nhịp điệu đọc tốt hơn, miễn là không làm mất ý nghĩa gốc.
-Hãy chuyển các yếu tố văn hóa Hàn Quốc một cách tự nhiên, giúp người đọc Việt Nam cảm nhận được sự gần gũi.
-Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản. 
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...)
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>You are an experienced literary editor specializing in processing and enhancing the quality of Vietnamese novels into English.
-Please translate the following text from Vietnamese to English with an engaging, smooth, and emotionally rich writing style.
-{count_info}
-Prioritize the naturalness and beauty of the English language over literal sentence-by-sentence translation.
-Use rich vocabulary, avoid repetition, and strive to convey the emotions within the text.
-Maintain the original numbering format (1., 2., ...)
-Here is the text to be translated:
-{text}</t>
-  </si>
-  <si>
-    <t>acc_original</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và dịch thuật các tác phẩm văn học Trung Quốc sang tiếng Việt. 
+Không thêm bớt, không làm thay đổi ý nghĩa của văn bản gốc, tránh diễn giải theo ý riêng. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và dịch thuật các tác phẩm văn học Trung Quốc sang tiếng Việt. 
 Hãy chuyển ngữ văn bản sau đây từ tiếng Trung sang tiếng Việt với độ chính xác cao, giữ gần nhất có thể với văn phong và cấu trúc nguyên gốc. 
-{count_info} 
 Dịch sát nghĩa từng câu, truyền tải đầy đủ thông tin từ bản gốc. 
 Giữ nguyên các tham chiếu văn hóa và thuật ngữ đặc thù mà không cần địa phương hóa quá mức. 
 Không thêm bớt, không làm thay đổi ý nghĩa của văn bản gốc, tránh diễn giải theo ý riêng. 
 Đối với tên nhân vật, hãy chuyển sang phiên âm Hán-Việt, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. Xưng hô giữa các nhân vật sử dụng 'ta, ngươi, hắn, cô ấy,...'.
 Phải dịch TOÀN BỘ văn bản sang tiếng Việt, không được để sót bất kỳ từ/câu tiếng Trung nào chưa dịch.
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...)
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>loose_original</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các tác phẩm văn học Trung Quốc sang tiếng Việt. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các tác phẩm văn học Trung Quốc sang tiếng Việt. 
 Hãy chuyển ngữ văn bản sau đây từ tiếng Trung sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
-{count_info} 
 Ưu tiên sự tự nhiên và vẻ đẹp của ngôn ngữ tiếng Việt hơn là dịch sát nghĩa từng câu. Bạn có thể điều chỉnh cấu trúc câu để tạo nhịp điệu đọc tốt hơn, miễn là không làm mất ý nghĩa gốc. 
 Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản. 
 Đối với tên nhân vật, hãy chuyển sang phiên âm Hán-Việt, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. Xưng hô giữa các nhân vật sử dụng 'ta, ngươi, hắn, cô ấy,...'.
 Phải dịch TOÀN BỘ văn bản sang tiếng Việt, không được để sót bất kỳ từ/câu tiếng Trung nào chưa dịch.
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...) 
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng văn học nước ngoài sang tiếng Việt. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng văn học nước ngoài sang tiếng Việt. 
 Hãy chuyển ngữ văn bản sau đây từ tiếng Anh sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
-{count_info} 
 Ưu tiên sự tự nhiên và vẻ đẹp của ngôn ngữ tiếng Việt hơn là dịch sát nghĩa từng câu. 
 Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản. 
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...)
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
+</t>
   </si>
   <si>
     <t xml:space="preserve">
 Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các tác phẩm văn học Hàn Quốc sang tiếng Việt. 
 Hãy chuyển ngữ văn bản sau đây từ tiếng Hàn sang tiếng Việt với văn phong tự nhiên, dễ đọc nhưng vẫn đảm bảo tính chính xác của nội dung gốc. 
-{count_info} 
 Cân bằng giữa sự mượt mà của ngôn ngữ tiếng Việt và việc truyền tải chính xác ý nghĩa từ bản gốc. Nếu có từ ngữ hoặc cụm từ mang tính văn hóa đặc trưng của Hàn Quốc, hãy giữ nguyên và chú thích ngắn gọn nếu cần thiết. 
 Đối với tên nhân vật, hãy chuyển sang phát âm tiếng Hàn, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
 Bạn có thể điều chỉnh cấu trúc câu một cách hợp lý để tạo nhịp điệu đọc tự nhiên trong tiếng Việt, miễn là không làm thay đổi ý nghĩa hoặc bối cảnh gốc. 
 Sử dụng ngôn từ phong phú và đa dạng, tránh lặp từ nhưng không quá cầu kỳ đến mức làm mất đi phong cách của tác giả. Truyền tải cảm xúc và không khí của văn bản gốc một cách tự nhiên. 
 Vẫn giữ định dạng đánh số và cấu trúc đoạn văn như bản gốc (1., 2., ...)
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>KR_loose</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các tác phẩm văn học từ tiếng Trung sang tiếng Việt, đặc biệt là với các tác phẩm gốc Hàn Quốc đã được dịch sang tiếng Trung. 
+</t>
+  </si>
+  <si>
+    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và dịch thuật các light novel Nhật Bản sang tiếng Việt. 
+Hãy chuyển ngữ văn bản sau đây từ tiếng Nhật sang tiếng Việt với độ chính xác cao, giữ gần nhất có thể với văn phong và cấu trúc nguyên gốc. 
+ Ưu tiên tính chính xác và trung thành với nội dung gốc. Cố gắng giữ nguyên cách diễn đạt, nhịp điệu và phong cách của tác giả. 
+Giữ nguyên các tham chiếu văn hóa và thuật ngữ đặc thù mà không cần địa phương hóa quá mức. 
+Giữ nguyên các hậu tố xưng hô như -san, -kun, -chan, -sama, -sensei, v.v. nếu có trong bản gốc
+Không thêm bớt, không làm thay đổi ý nghĩa của văn bản gốc, tránh diễn giải theo ý riêng. 
+Phải dịch TOÀN BỘ văn bản sang tiếng Việt, không được để sót bất kỳ từ/câu tiếng Nhật nào chưa dịch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và dịch thuật các tác phẩm văn học tiếng Anh sang tiếng Việt. 
+Hãy chuyển ngữ văn bản sau đây từ tiếng Anh sang tiếng Việt với độ chính xác cao, giữ gần nhất có thể với văn phong và cấu trúc nguyên gốc. 
+ Dịch sát nghĩa từng câu, truyền tải đầy đủ thông tin từ bản gốc. 
+Giữ nguyên tên nhân vật, địa danh và các thuật ngữ đặc thù như trong bản gốc tiếng Anh.
+Các thành ngữ, tục ngữ tiếng Anh cần được dịch sang những biểu đạt tương đương trong tiếng Việt nếu có.
+Không thêm bớt, không làm thay đổi ý nghĩa của văn bản gốc, tránh diễn giải theo ý riêng. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và dịch thuật các tác phẩm văn học Hàn Quốc sang tiếng Việt. 
+Hãy chuyển ngữ văn bản sau đây từ tiếng Hàn sang tiếng Việt với độ chính xác cao, giữ gần nhất có thể với văn phong và cấu trúc nguyên gốc. 
+ Dịch sát nghĩa từng câu, truyền tải đầy đủ thông tin từ bản gốc. 
+Đối với tên nhân vật, hãy chuyển sang phiên âm tiếng Việt theo cách đọc tiếng Hàn.
+Các thuật ngữ đặc trưng văn hóa Hàn Quốc hãy giữ nguyên và thêm giải thích ngắn nếu cần thiết.
+Các mức độ kính ngữ trong tiếng Hàn cần được chuyển thành biểu đạt tương ứng với ngôn ngữ tiếng Việt.
+Không thêm bớt, không làm thay đổi ý nghĩa của văn bản gốc, tránh diễn giải theo ý riêng. </t>
+  </si>
+  <si>
+    <t>You are an experienced literary editor specializing in processing and translating Vietnamese literary works into English.
+Please translate the following text from Vietnamese to English with high accuracy, maintaining as closely as possible the original style and structure.
+Translate each sentence faithfully, conveying complete information from the original text.
+Preserve character names, place names, and specific terminology as they appear in the original Vietnamese.
+Vietnamese idioms and proverbs should be translated into equivalent English expressions where available.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are an experienced literary editor specializing in processing and enhancing the quality of Vietnamese novels into English.
+Please translate the following text from Vietnamese to English with an engaging, smooth, and emotionally rich writing style.
+Prioritize the naturalness and beauty of the English language over literal sentence-by-sentence translation.
+Use rich vocabulary, avoid repetition, and strive to convey the emotions within the text.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các tác phẩm văn học Hàn Quốc sang tiếng Việt. 
+Hãy chuyển ngữ văn bản sau đây từ tiếng Hàn sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
+ Ưu tiên sự tự nhiên và vẻ đẹp của ngôn ngữ tiếng Việt hơn là dịch sát nghĩa từng câu. 
+Đối với tên nhân vật, hãy chuyển sang phiên âm tiếng Việt theo cách đọc tiếng Hàn, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
+Bạn có thể điều chỉnh cấu trúc câu để tạo nhịp điệu đọc tốt hơn, miễn là không làm mất ý nghĩa gốc.
+Hãy chuyển các yếu tố văn hóa Hàn Quốc một cách tự nhiên, giúp người đọc Việt Nam cảm nhận được sự gần gũi.
+Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
+Hãy chuyển ngữ văn bản sau đây từ tiếng Trung sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
+ Ưu tiên sự tự nhiên và vẻ đẹp của ngôn ngữ tiếng Việt hơn là dịch sát nghĩa từng câu. 
+Đối với tên nhân vật, hãy chuyển sang phát âm tiếng Nhật, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
+Bạn có thể điều chỉnh cấu trúc câu để tạo nhịp điệu đọc tốt hơn, miễn là không làm mất ý nghĩa gốc. 
+Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản. </t>
+  </si>
+  <si>
+    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
+Hãy chuyển ngữ văn bản sau đây từ tiếng Nhật sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
+ Ưu tiên sự tự nhiên và vẻ đẹp của ngôn ngữ tiếng Việt hơn là dịch sát nghĩa từng câu. 
+Đối với tên nhân vật, hãy chuyển sang phát âm tiếng Nhật, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
+Bạn có thể điều chỉnh cấu trúc câu để tạo nhịp điệu đọc tốt hơn, miễn là không làm mất ý nghĩa gốc.
+Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản. 
+Phải dịch TOÀN BỘ văn bản sang tiếng Việt, không được để sót bất kỳ từ/câu tiếng Nhật nào chưa dịch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các light novel Nhật Bản sang tiếng Việt. 
+Hãy chuyển ngữ văn bản sau đây từ tiếng Anh sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc. 
+ Ưu tiên sự tự nhiên và vẻ đẹp của ngôn ngữ tiếng Việt hơn là dịch sát nghĩa từng câu. 
+Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải cảm xúc trong văn bản. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các tác phẩm văn học từ tiếng Trung sang tiếng Việt, đặc biệt là với các tác phẩm gốc Hàn Quốc đã được dịch sang tiếng Trung. 
 Hãy chuyển ngữ văn bản sau đây từ tiếng Trung sang tiếng Việt với văn phong hấp dẫn, mượt mà và giàu cảm xúc, nhưng vẫn đảm bảo tính chính xác của nội dung gốc. 
-{count_info} 
-Đối với tên nhân vật Hàn Quốc, hãy chuyển về cách viết tên theo tiếng Hàn chính xác (nếu có thể xác định), hoặc sử dụng cách phiên âm tiếng Hàn phổ biến thay vì phiên âm Hán-Việt. Với tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
-Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải đúng cảm xúc và phong cách văn học Hàn Quốc. 
-Vẫn giữ định dạng đánh số như bản gốc (1., 2., ...) 
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>KR_acc</t>
-  </si>
-  <si>
-    <t>Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các tác phẩm văn học Hàn Quốc sang tiếng Việt. 
+ Đối với tên nhân vật Hàn Quốc, hãy chuyển về cách viết tên theo tiếng Hàn chính xác (nếu có thể xác định), hoặc sử dụng cách phiên âm tiếng Hàn phổ biến thay vì phiên âm Hán-Việt. Với tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
+Hãy sử dụng ngôn từ phong phú, tránh lặp từ và cố gắng truyền tải đúng cảm xúc và phong cách văn học Hàn Quốc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là một biên tập viên văn học đầy kinh nghiệm, chuyên xử lý và nâng cao chất lượng các tác phẩm văn học Hàn Quốc sang tiếng Việt. 
 Hãy chuyển ngữ văn bản sau đây từ tiếng Hàn sang tiếng Việt với văn phong tự nhiên, dễ đọc nhưng vẫn đảm bảo tính chính xác của nội dung gốc. 
-{count_info} 
 Cân bằng giữa sự mượt mà của ngôn ngữ tiếng Việt và việc truyền tải chính xác ý nghĩa từ bản gốc.
 Đối với tên nhân vật, hãy chuyển sang phát âm tiếng Hàn, trừ những tên tiếng Anh hoặc ngôn ngữ phổ biến khác thì giữ nguyên. 
 Bạn có thể điều chỉnh cấu trúc câu một cách hợp lý để tạo nhịp điệu đọc tự nhiên trong tiếng Việt, miễn là không làm thay đổi ý nghĩa hoặc bối cảnh gốc. 
 Sử dụng ngôn từ phong phú và đa dạng, tránh lặp từ nhưng không quá cầu kỳ đến mức làm mất đi phong cách của tác giả. Truyền tải cảm xúc và không khí của văn bản gốc một cách tự nhiên. 
-Vẫn giữ định dạng đánh số và cấu trúc đoạn văn như bản gốc (1., 2., ...)
-Đây là văn bản cần chuyển ngữ:
-{text}</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>You are a master literary translator and accomplished author with decades of experience in both Vietnamese and English literature. Your translations read as if originally written by a native English-speaking novelist.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are a master literary translator and accomplished author with decades of experience in both Vietnamese and English literature. Your translations read as if originally written by a native English-speaking novelist.
 Transform the following Vietnamese text into exquisite English prose that captures not just the meaning, but the soul and rhythm of the original work.
-{count_info}
 **Your approach:**
 - Write as a professional author would, not as a translator
 - Craft sentences that flow naturally and beautifully in English
@@ -271,7 +211,7 @@
 - Maintain paragraph structure and dialogue formatting
 Your goal is to create a translation so polished and engaging that readers forget they're reading a translated work. Make every sentence sing in English while honoring the Vietnamese original.
 Here is the text to transform:
-{text}</t>
+</t>
   </si>
 </sst>
 </file>
@@ -327,10 +267,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -637,7 +580,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,89 +608,89 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>